<commit_message>
Se Añadio sintaxis para graficar  el Genero, Edad, Ciclo y Ecuela Profesional
</commit_message>
<xml_diff>
--- a/BDTesis-DLA.xlsx
+++ b/BDTesis-DLA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OLID JP\GitHub Repositorio\Practicando-R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FC322E-0E67-474A-9681-C5BEBC8DDB97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685D3C37-A270-4322-9C55-760A955A96A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E572D2CA-CBE9-48EC-9257-4C40B3DF4F72}"/>
   </bookViews>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Ciclo</t>
-  </si>
-  <si>
-    <t>Escuala Profesional</t>
   </si>
   <si>
     <t>ITEM01</t>
@@ -241,6 +238,9 @@
   </si>
   <si>
     <t>Femenino</t>
+  </si>
+  <si>
+    <t>Escuela Profesional</t>
   </si>
 </sst>
 </file>
@@ -618,7 +618,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E9DA61E-90FB-4AB3-983D-FE90D47EE1BB}">
   <dimension ref="A1:AX302"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -639,142 +641,142 @@
         <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
@@ -782,7 +784,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="2">
         <v>20</v>
@@ -934,7 +936,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="2">
         <v>20</v>
@@ -1086,7 +1088,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="2">
         <v>18</v>
@@ -1238,7 +1240,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" s="2">
         <v>17</v>
@@ -1390,7 +1392,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="2">
         <v>18</v>
@@ -1542,7 +1544,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="2">
         <v>19</v>
@@ -1694,7 +1696,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="2">
         <v>18</v>
@@ -1846,7 +1848,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="2">
         <v>19</v>
@@ -1998,7 +2000,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="2">
         <v>17</v>
@@ -2150,7 +2152,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" s="2">
         <v>19</v>
@@ -2302,7 +2304,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" s="2">
         <v>18</v>
@@ -2454,7 +2456,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="2">
         <v>17</v>
@@ -2606,7 +2608,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" s="2">
         <v>19</v>
@@ -2758,7 +2760,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="2">
         <v>18</v>
@@ -2910,7 +2912,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="2">
         <v>18</v>
@@ -3062,7 +3064,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="2">
         <v>20</v>
@@ -3214,7 +3216,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" s="2">
         <v>19</v>
@@ -3366,7 +3368,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="2">
         <v>21</v>
@@ -3518,7 +3520,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="2">
         <v>20</v>
@@ -3670,7 +3672,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="2">
         <v>20</v>
@@ -3822,7 +3824,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22" s="2">
         <v>26</v>
@@ -3974,7 +3976,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23" s="2">
         <v>25</v>
@@ -4126,7 +4128,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C24" s="2">
         <v>22</v>
@@ -4278,7 +4280,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C25" s="2">
         <v>26</v>
@@ -4430,7 +4432,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="2">
         <v>18</v>
@@ -4582,7 +4584,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C27" s="2">
         <v>23</v>
@@ -4734,7 +4736,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C28" s="2">
         <v>26</v>
@@ -4886,7 +4888,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="2">
         <v>19</v>
@@ -5038,7 +5040,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="2">
         <v>18</v>
@@ -5190,7 +5192,7 @@
         <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C31" s="2">
         <v>27</v>
@@ -5342,7 +5344,7 @@
         <v>2</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="2">
         <v>20</v>
@@ -5494,7 +5496,7 @@
         <v>3</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C33" s="2">
         <v>22</v>
@@ -5646,7 +5648,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C34" s="2">
         <v>18</v>
@@ -5798,7 +5800,7 @@
         <v>5</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C35" s="2">
         <v>19</v>
@@ -5950,7 +5952,7 @@
         <v>6</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C36" s="2">
         <v>24</v>
@@ -6102,7 +6104,7 @@
         <v>7</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C37" s="2">
         <v>19</v>
@@ -6254,7 +6256,7 @@
         <v>8</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C38" s="2">
         <v>19</v>
@@ -6406,7 +6408,7 @@
         <v>9</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C39" s="2">
         <v>18</v>
@@ -6558,7 +6560,7 @@
         <v>10</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C40" s="2">
         <v>19</v>
@@ -6710,7 +6712,7 @@
         <v>11</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C41" s="2">
         <v>18</v>
@@ -6862,7 +6864,7 @@
         <v>12</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C42" s="2">
         <v>18</v>
@@ -7014,7 +7016,7 @@
         <v>13</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C43" s="2">
         <v>21</v>
@@ -7166,7 +7168,7 @@
         <v>14</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C44" s="2">
         <v>22</v>
@@ -7318,7 +7320,7 @@
         <v>15</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C45" s="2">
         <v>25</v>
@@ -7470,7 +7472,7 @@
         <v>16</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C46" s="2">
         <v>27</v>
@@ -7622,7 +7624,7 @@
         <v>17</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C47" s="2">
         <v>26</v>
@@ -7774,7 +7776,7 @@
         <v>18</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C48" s="2">
         <v>23</v>
@@ -7926,7 +7928,7 @@
         <v>19</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C49" s="2">
         <v>24</v>
@@ -8078,7 +8080,7 @@
         <v>20</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C50" s="2">
         <v>22</v>
@@ -8230,7 +8232,7 @@
         <v>21</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C51" s="2">
         <v>24</v>
@@ -8382,7 +8384,7 @@
         <v>22</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C52" s="2">
         <v>25</v>
@@ -8534,7 +8536,7 @@
         <v>23</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C53" s="2">
         <v>26</v>
@@ -8686,7 +8688,7 @@
         <v>24</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C54" s="2">
         <v>24</v>
@@ -8838,7 +8840,7 @@
         <v>25</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C55" s="2">
         <v>24</v>
@@ -8990,7 +8992,7 @@
         <v>26</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C56" s="2">
         <v>22</v>
@@ -9142,7 +9144,7 @@
         <v>27</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C57" s="2">
         <v>20</v>
@@ -9294,7 +9296,7 @@
         <v>28</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C58" s="2">
         <v>22</v>
@@ -9446,7 +9448,7 @@
         <v>29</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C59" s="2">
         <v>26</v>
@@ -9598,7 +9600,7 @@
         <v>30</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C60" s="2">
         <v>25</v>
@@ -9750,7 +9752,7 @@
         <v>31</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C61" s="2">
         <v>23</v>
@@ -9902,7 +9904,7 @@
         <v>32</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C62" s="2">
         <v>24</v>
@@ -10054,7 +10056,7 @@
         <v>33</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C63" s="2">
         <v>24</v>
@@ -10206,7 +10208,7 @@
         <v>34</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C64" s="2">
         <v>25</v>
@@ -10358,7 +10360,7 @@
         <v>35</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C65" s="2">
         <v>27</v>
@@ -10510,7 +10512,7 @@
         <v>36</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C66" s="2">
         <v>22</v>
@@ -10662,7 +10664,7 @@
         <v>37</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C67" s="2">
         <v>24</v>
@@ -10814,7 +10816,7 @@
         <v>38</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C68" s="2">
         <v>24</v>
@@ -10966,7 +10968,7 @@
         <v>1</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C69" s="2">
         <v>30</v>
@@ -11118,7 +11120,7 @@
         <v>2</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C70" s="2">
         <v>23</v>
@@ -11270,7 +11272,7 @@
         <v>3</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C71" s="2">
         <v>28</v>
@@ -11422,7 +11424,7 @@
         <v>4</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C72" s="2">
         <v>30</v>
@@ -11574,7 +11576,7 @@
         <v>5</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C73" s="2">
         <v>27</v>
@@ -11726,7 +11728,7 @@
         <v>6</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C74" s="2">
         <v>24</v>
@@ -11878,7 +11880,7 @@
         <v>7</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C75" s="2">
         <v>26</v>
@@ -12030,7 +12032,7 @@
         <v>8</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C76" s="2">
         <v>27</v>
@@ -12182,7 +12184,7 @@
         <v>1</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C77" s="2">
         <v>22</v>
@@ -12334,7 +12336,7 @@
         <v>2</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C78" s="2">
         <v>22</v>
@@ -12486,7 +12488,7 @@
         <v>3</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C79" s="2">
         <v>20</v>
@@ -12638,7 +12640,7 @@
         <v>4</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C80" s="2">
         <v>20</v>
@@ -12790,7 +12792,7 @@
         <v>5</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C81" s="2">
         <v>27</v>
@@ -12942,7 +12944,7 @@
         <v>6</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C82" s="2">
         <v>18</v>
@@ -13094,7 +13096,7 @@
         <v>7</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C83" s="2">
         <v>21</v>
@@ -13246,7 +13248,7 @@
         <v>8</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C84" s="2">
         <v>21</v>
@@ -13398,7 +13400,7 @@
         <v>9</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C85" s="2">
         <v>19</v>
@@ -13550,7 +13552,7 @@
         <v>10</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C86" s="2">
         <v>20</v>
@@ -13702,7 +13704,7 @@
         <v>11</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C87" s="2">
         <v>19</v>
@@ -13854,7 +13856,7 @@
         <v>12</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C88" s="2">
         <v>18</v>
@@ -14006,7 +14008,7 @@
         <v>13</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C89" s="2">
         <v>19</v>
@@ -14158,7 +14160,7 @@
         <v>14</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C90" s="2">
         <v>19</v>
@@ -14310,7 +14312,7 @@
         <v>15</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C91" s="2">
         <v>24</v>
@@ -14462,7 +14464,7 @@
         <v>16</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C92" s="2">
         <v>21</v>
@@ -14614,7 +14616,7 @@
         <v>17</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C93" s="2">
         <v>20</v>
@@ -14766,7 +14768,7 @@
         <v>18</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C94" s="2">
         <v>18</v>
@@ -14918,7 +14920,7 @@
         <v>19</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C95" s="2">
         <v>20</v>
@@ -15070,7 +15072,7 @@
         <v>20</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C96" s="2">
         <v>19</v>
@@ -15222,7 +15224,7 @@
         <v>21</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C97" s="2">
         <v>20</v>
@@ -15374,7 +15376,7 @@
         <v>22</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C98" s="2">
         <v>19</v>
@@ -15526,7 +15528,7 @@
         <v>23</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C99" s="2">
         <v>20</v>
@@ -15678,7 +15680,7 @@
         <v>24</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C100" s="2">
         <v>19</v>
@@ -15830,7 +15832,7 @@
         <v>25</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C101" s="2">
         <v>20</v>
@@ -15982,7 +15984,7 @@
         <v>26</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C102" s="2">
         <v>25</v>
@@ -16134,7 +16136,7 @@
         <v>27</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C103" s="2">
         <v>19</v>
@@ -16286,7 +16288,7 @@
         <v>28</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C104" s="2">
         <v>20</v>
@@ -16438,7 +16440,7 @@
         <v>29</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C105" s="2">
         <v>18</v>
@@ -16590,7 +16592,7 @@
         <v>30</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C106" s="2">
         <v>20</v>
@@ -16742,7 +16744,7 @@
         <v>31</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C107" s="2">
         <v>26</v>
@@ -16894,7 +16896,7 @@
         <v>32</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C108" s="2">
         <v>25</v>
@@ -17046,7 +17048,7 @@
         <v>33</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C109" s="2">
         <v>19</v>
@@ -17198,7 +17200,7 @@
         <v>34</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C110" s="2">
         <v>20</v>
@@ -17350,7 +17352,7 @@
         <v>35</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C111" s="2">
         <v>20</v>
@@ -17502,7 +17504,7 @@
         <v>36</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C112" s="2">
         <v>21</v>
@@ -17654,7 +17656,7 @@
         <v>37</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C113" s="2">
         <v>19</v>
@@ -17806,7 +17808,7 @@
         <v>38</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C114" s="2">
         <v>18</v>
@@ -17958,7 +17960,7 @@
         <v>39</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C115" s="2">
         <v>22</v>
@@ -18110,7 +18112,7 @@
         <v>40</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C116" s="2">
         <v>19</v>
@@ -18262,7 +18264,7 @@
         <v>41</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C117" s="2">
         <v>23</v>
@@ -18414,7 +18416,7 @@
         <v>42</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C118" s="2">
         <v>20</v>
@@ -18566,7 +18568,7 @@
         <v>43</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C119" s="2">
         <v>18</v>
@@ -18718,7 +18720,7 @@
         <v>44</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C120" s="2">
         <v>20</v>
@@ -18870,7 +18872,7 @@
         <v>45</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C121" s="2">
         <v>21</v>
@@ -19022,7 +19024,7 @@
         <v>46</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C122" s="2">
         <v>24</v>
@@ -19174,7 +19176,7 @@
         <v>1</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C123" s="2">
         <v>23</v>
@@ -19326,7 +19328,7 @@
         <v>2</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C124" s="2">
         <v>25</v>
@@ -19478,7 +19480,7 @@
         <v>3</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C125" s="2">
         <v>25</v>
@@ -19630,7 +19632,7 @@
         <v>4</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C126" s="2">
         <v>21</v>
@@ -19782,7 +19784,7 @@
         <v>5</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C127" s="2">
         <v>21</v>
@@ -19934,7 +19936,7 @@
         <v>6</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C128" s="2">
         <v>21</v>
@@ -20086,7 +20088,7 @@
         <v>7</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C129" s="2">
         <v>23</v>
@@ -20238,7 +20240,7 @@
         <v>8</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C130" s="2">
         <v>21</v>
@@ -20390,7 +20392,7 @@
         <v>9</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C131" s="2">
         <v>20</v>
@@ -20542,7 +20544,7 @@
         <v>10</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C132" s="2">
         <v>22</v>
@@ -20694,7 +20696,7 @@
         <v>11</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C133" s="2">
         <v>21</v>
@@ -20846,7 +20848,7 @@
         <v>12</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C134" s="2">
         <v>19</v>
@@ -20998,7 +21000,7 @@
         <v>13</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C135" s="2">
         <v>21</v>
@@ -21150,7 +21152,7 @@
         <v>14</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C136" s="2">
         <v>19</v>
@@ -21302,7 +21304,7 @@
         <v>15</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C137" s="2">
         <v>21</v>
@@ -21454,7 +21456,7 @@
         <v>16</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C138" s="2">
         <v>20</v>
@@ -21606,7 +21608,7 @@
         <v>17</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C139" s="2">
         <v>20</v>
@@ -21758,7 +21760,7 @@
         <v>18</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C140" s="2">
         <v>21</v>
@@ -21910,7 +21912,7 @@
         <v>19</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C141" s="2">
         <v>19</v>
@@ -22062,7 +22064,7 @@
         <v>20</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C142" s="2">
         <v>20</v>
@@ -22214,7 +22216,7 @@
         <v>21</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C143" s="2">
         <v>19</v>
@@ -22366,7 +22368,7 @@
         <v>22</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C144" s="2">
         <v>23</v>
@@ -22518,7 +22520,7 @@
         <v>23</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C145" s="2">
         <v>21</v>
@@ -22670,7 +22672,7 @@
         <v>24</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C146" s="2">
         <v>19</v>
@@ -22822,7 +22824,7 @@
         <v>25</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C147" s="2">
         <v>24</v>
@@ -22974,7 +22976,7 @@
         <v>26</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C148" s="2">
         <v>19</v>
@@ -23126,7 +23128,7 @@
         <v>27</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C149" s="2">
         <v>20</v>
@@ -23278,7 +23280,7 @@
         <v>28</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C150" s="2">
         <v>19</v>
@@ -23430,7 +23432,7 @@
         <v>29</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C151" s="2">
         <v>20</v>
@@ -23582,7 +23584,7 @@
         <v>30</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C152" s="2">
         <v>21</v>
@@ -23734,7 +23736,7 @@
         <v>31</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C153" s="2">
         <v>18</v>
@@ -23886,7 +23888,7 @@
         <v>32</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C154" s="2">
         <v>21</v>
@@ -24038,7 +24040,7 @@
         <v>33</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C155" s="2">
         <v>22</v>
@@ -24190,7 +24192,7 @@
         <v>34</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C156" s="2">
         <v>18</v>
@@ -24342,7 +24344,7 @@
         <v>35</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C157" s="2">
         <v>21</v>
@@ -24494,7 +24496,7 @@
         <v>36</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C158" s="2">
         <v>22</v>
@@ -24646,7 +24648,7 @@
         <v>37</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C159" s="2">
         <v>23</v>
@@ -24798,7 +24800,7 @@
         <v>38</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C160" s="2">
         <v>21</v>
@@ -24950,7 +24952,7 @@
         <v>39</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C161" s="2">
         <v>21</v>
@@ -25102,7 +25104,7 @@
         <v>40</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C162" s="2">
         <v>20</v>
@@ -25254,7 +25256,7 @@
         <v>41</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C163" s="2">
         <v>23</v>
@@ -25406,7 +25408,7 @@
         <v>42</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C164" s="2">
         <v>21</v>
@@ -25558,7 +25560,7 @@
         <v>43</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C165" s="2">
         <v>23</v>
@@ -25710,7 +25712,7 @@
         <v>44</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C166" s="2">
         <v>19</v>
@@ -25862,7 +25864,7 @@
         <v>45</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C167" s="2">
         <v>20</v>
@@ -26014,7 +26016,7 @@
         <v>46</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C168" s="2">
         <v>22</v>
@@ -26166,7 +26168,7 @@
         <v>47</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C169" s="2">
         <v>21</v>
@@ -26318,7 +26320,7 @@
         <v>48</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C170" s="2">
         <v>23</v>
@@ -26470,7 +26472,7 @@
         <v>49</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C171" s="2">
         <v>23</v>
@@ -26622,7 +26624,7 @@
         <v>50</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C172" s="2">
         <v>20</v>
@@ -26774,7 +26776,7 @@
         <v>51</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C173" s="2">
         <v>22</v>
@@ -26926,7 +26928,7 @@
         <v>1</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C174" s="2">
         <v>32</v>
@@ -27078,7 +27080,7 @@
         <v>2</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C175" s="2">
         <v>20</v>
@@ -27230,7 +27232,7 @@
         <v>3</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C176" s="2">
         <v>19</v>
@@ -27382,7 +27384,7 @@
         <v>4</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C177" s="2">
         <v>18</v>
@@ -27534,7 +27536,7 @@
         <v>5</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C178" s="2">
         <v>19</v>
@@ -27686,7 +27688,7 @@
         <v>6</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C179" s="2">
         <v>22</v>
@@ -27838,7 +27840,7 @@
         <v>7</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C180" s="2">
         <v>19</v>
@@ -27990,7 +27992,7 @@
         <v>8</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C181" s="2">
         <v>21</v>
@@ -28142,7 +28144,7 @@
         <v>9</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C182" s="2">
         <v>19</v>
@@ -28294,7 +28296,7 @@
         <v>10</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C183" s="2">
         <v>19</v>
@@ -28446,7 +28448,7 @@
         <v>11</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C184" s="2">
         <v>22</v>
@@ -28598,7 +28600,7 @@
         <v>12</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C185" s="2">
         <v>18</v>
@@ -28750,7 +28752,7 @@
         <v>13</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C186" s="2">
         <v>20</v>
@@ -28902,7 +28904,7 @@
         <v>14</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C187" s="2">
         <v>20</v>
@@ -29054,7 +29056,7 @@
         <v>15</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C188" s="2">
         <v>20</v>
@@ -29206,7 +29208,7 @@
         <v>16</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C189" s="2">
         <v>18</v>
@@ -29358,7 +29360,7 @@
         <v>17</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C190" s="2">
         <v>18</v>
@@ -29510,7 +29512,7 @@
         <v>18</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C191" s="2">
         <v>19</v>
@@ -29662,7 +29664,7 @@
         <v>19</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C192" s="2">
         <v>18</v>
@@ -29814,7 +29816,7 @@
         <v>20</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C193" s="2">
         <v>23</v>
@@ -29966,7 +29968,7 @@
         <v>21</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C194" s="2">
         <v>19</v>
@@ -30118,7 +30120,7 @@
         <v>22</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C195" s="2">
         <v>18</v>
@@ -30270,7 +30272,7 @@
         <v>23</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C196" s="2">
         <v>18</v>
@@ -30422,7 +30424,7 @@
         <v>24</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C197" s="2">
         <v>18</v>
@@ -30574,7 +30576,7 @@
         <v>25</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C198" s="2">
         <v>26</v>
@@ -30726,7 +30728,7 @@
         <v>26</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C199" s="2">
         <v>24</v>
@@ -30878,7 +30880,7 @@
         <v>27</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C200" s="2">
         <v>24</v>
@@ -31030,7 +31032,7 @@
         <v>28</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C201" s="2">
         <v>24</v>
@@ -31182,7 +31184,7 @@
         <v>29</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C202" s="2">
         <v>21</v>
@@ -31334,7 +31336,7 @@
         <v>30</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C203" s="2">
         <v>23</v>
@@ -31486,7 +31488,7 @@
         <v>31</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C204" s="2">
         <v>24</v>
@@ -31638,7 +31640,7 @@
         <v>32</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C205" s="2">
         <v>21</v>
@@ -31790,7 +31792,7 @@
         <v>33</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C206" s="2">
         <v>18</v>
@@ -31942,7 +31944,7 @@
         <v>34</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C207" s="2">
         <v>23</v>
@@ -32094,7 +32096,7 @@
         <v>35</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C208" s="2">
         <v>24</v>
@@ -32246,7 +32248,7 @@
         <v>36</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C209" s="2">
         <v>24</v>
@@ -32398,7 +32400,7 @@
         <v>37</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C210" s="2">
         <v>18</v>
@@ -32550,7 +32552,7 @@
         <v>38</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C211" s="2">
         <v>22</v>
@@ -32702,7 +32704,7 @@
         <v>39</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C212" s="2">
         <v>23</v>
@@ -32854,7 +32856,7 @@
         <v>40</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C213" s="2">
         <v>24</v>
@@ -33006,7 +33008,7 @@
         <v>41</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C214" s="2">
         <v>23</v>
@@ -33158,7 +33160,7 @@
         <v>42</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C215" s="2">
         <v>24</v>
@@ -33310,7 +33312,7 @@
         <v>43</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C216" s="2">
         <v>23</v>
@@ -33462,7 +33464,7 @@
         <v>44</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C217" s="2">
         <v>21</v>
@@ -33614,7 +33616,7 @@
         <v>45</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C218" s="2">
         <v>18</v>
@@ -33766,7 +33768,7 @@
         <v>46</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C219" s="2">
         <v>18</v>
@@ -33918,7 +33920,7 @@
         <v>47</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C220" s="2">
         <v>20</v>
@@ -34070,7 +34072,7 @@
         <v>48</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C221" s="2">
         <v>24</v>
@@ -34222,7 +34224,7 @@
         <v>49</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C222" s="2">
         <v>20</v>
@@ -34374,7 +34376,7 @@
         <v>50</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C223" s="2">
         <v>19</v>
@@ -34526,7 +34528,7 @@
         <v>51</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C224" s="2">
         <v>22</v>
@@ -34678,7 +34680,7 @@
         <v>52</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C225" s="2">
         <v>23</v>
@@ -34830,7 +34832,7 @@
         <v>53</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C226" s="2">
         <v>24</v>
@@ -34982,7 +34984,7 @@
         <v>54</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C227" s="2">
         <v>23</v>
@@ -35134,7 +35136,7 @@
         <v>55</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C228" s="2">
         <v>25</v>
@@ -35286,7 +35288,7 @@
         <v>56</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C229" s="2">
         <v>24</v>
@@ -35438,7 +35440,7 @@
         <v>57</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C230" s="2">
         <v>25</v>
@@ -35590,7 +35592,7 @@
         <v>58</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C231" s="2">
         <v>22</v>
@@ -35742,7 +35744,7 @@
         <v>59</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C232" s="2">
         <v>21</v>
@@ -35894,7 +35896,7 @@
         <v>60</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C233" s="2">
         <v>24</v>
@@ -36046,7 +36048,7 @@
         <v>61</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C234" s="2">
         <v>18</v>
@@ -36198,7 +36200,7 @@
         <v>62</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C235" s="2">
         <v>21</v>
@@ -36350,7 +36352,7 @@
         <v>63</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C236" s="2">
         <v>25</v>
@@ -36502,7 +36504,7 @@
         <v>64</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C237" s="2">
         <v>21</v>
@@ -36654,7 +36656,7 @@
         <v>65</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C238" s="2">
         <v>24</v>
@@ -36806,7 +36808,7 @@
         <v>66</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C239" s="2">
         <v>24</v>
@@ -36958,7 +36960,7 @@
         <v>67</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C240" s="2">
         <v>25</v>
@@ -37110,7 +37112,7 @@
         <v>68</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C241" s="2">
         <v>26</v>
@@ -37262,7 +37264,7 @@
         <v>69</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C242" s="2">
         <v>27</v>
@@ -37414,7 +37416,7 @@
         <v>70</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C243" s="2">
         <v>21</v>
@@ -37566,7 +37568,7 @@
         <v>71</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C244" s="2">
         <v>24</v>
@@ -37718,7 +37720,7 @@
         <v>72</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C245" s="2">
         <v>25</v>
@@ -37870,7 +37872,7 @@
         <v>73</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C246" s="2">
         <v>26</v>
@@ -38022,7 +38024,7 @@
         <v>74</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C247" s="2">
         <v>18</v>
@@ -38174,7 +38176,7 @@
         <v>75</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C248" s="2">
         <v>20</v>
@@ -38326,7 +38328,7 @@
         <v>76</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C249" s="2">
         <v>22</v>
@@ -38478,7 +38480,7 @@
         <v>77</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C250" s="2">
         <v>28</v>
@@ -38630,7 +38632,7 @@
         <v>78</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C251" s="2">
         <v>27</v>
@@ -38782,7 +38784,7 @@
         <v>79</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C252" s="2">
         <v>27</v>
@@ -38934,7 +38936,7 @@
         <v>80</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C253" s="2">
         <v>25</v>
@@ -39086,7 +39088,7 @@
         <v>81</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C254" s="2">
         <v>20</v>
@@ -39238,7 +39240,7 @@
         <v>82</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C255" s="2">
         <v>26</v>
@@ -39390,7 +39392,7 @@
         <v>83</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C256" s="2">
         <v>24</v>
@@ -39542,7 +39544,7 @@
         <v>84</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C257" s="2">
         <v>18</v>
@@ -39694,7 +39696,7 @@
         <v>85</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C258" s="2">
         <v>20</v>
@@ -39846,7 +39848,7 @@
         <v>86</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C259" s="2">
         <v>26</v>
@@ -39998,7 +40000,7 @@
         <v>87</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C260" s="2">
         <v>25</v>
@@ -40150,7 +40152,7 @@
         <v>88</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C261" s="2">
         <v>22</v>
@@ -40302,7 +40304,7 @@
         <v>89</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C262" s="2">
         <v>26</v>
@@ -40454,7 +40456,7 @@
         <v>90</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C263" s="2">
         <v>18</v>
@@ -40606,7 +40608,7 @@
         <v>91</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C264" s="2">
         <v>23</v>
@@ -40758,7 +40760,7 @@
         <v>92</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C265" s="2">
         <v>26</v>
@@ -40910,7 +40912,7 @@
         <v>93</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C266" s="2">
         <v>19</v>
@@ -41062,7 +41064,7 @@
         <v>1</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C267" s="2">
         <v>22</v>
@@ -41214,7 +41216,7 @@
         <v>2</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C268" s="2">
         <v>22</v>
@@ -41366,7 +41368,7 @@
         <v>3</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C269" s="2">
         <v>22</v>
@@ -41518,7 +41520,7 @@
         <v>4</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C270" s="2">
         <v>18</v>
@@ -41670,7 +41672,7 @@
         <v>5</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C271" s="2">
         <v>21</v>
@@ -41822,7 +41824,7 @@
         <v>6</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C272" s="2">
         <v>22</v>
@@ -41974,7 +41976,7 @@
         <v>7</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C273" s="2">
         <v>21</v>
@@ -42126,7 +42128,7 @@
         <v>8</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C274" s="2">
         <v>21</v>
@@ -42278,7 +42280,7 @@
         <v>9</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C275" s="2">
         <v>21</v>
@@ -42430,7 +42432,7 @@
         <v>10</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C276" s="2">
         <v>20</v>
@@ -42582,7 +42584,7 @@
         <v>11</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C277" s="2">
         <v>19</v>
@@ -42734,7 +42736,7 @@
         <v>12</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C278" s="2">
         <v>20</v>
@@ -42886,7 +42888,7 @@
         <v>13</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C279" s="2">
         <v>20</v>
@@ -43038,7 +43040,7 @@
         <v>14</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C280" s="2">
         <v>20</v>
@@ -43190,7 +43192,7 @@
         <v>15</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C281" s="2">
         <v>20</v>
@@ -43342,7 +43344,7 @@
         <v>16</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C282" s="2">
         <v>22</v>
@@ -43494,7 +43496,7 @@
         <v>17</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C283" s="2">
         <v>18</v>
@@ -43646,7 +43648,7 @@
         <v>18</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C284" s="2">
         <v>20</v>
@@ -43798,7 +43800,7 @@
         <v>19</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C285" s="2">
         <v>19</v>
@@ -43950,7 +43952,7 @@
         <v>20</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C286" s="2">
         <v>20</v>
@@ -44102,7 +44104,7 @@
         <v>21</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C287" s="2">
         <v>20</v>
@@ -44254,7 +44256,7 @@
         <v>22</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C288" s="2">
         <v>18</v>
@@ -44406,7 +44408,7 @@
         <v>23</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C289" s="2">
         <v>20</v>
@@ -44558,7 +44560,7 @@
         <v>24</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C290" s="2">
         <v>23</v>
@@ -44710,7 +44712,7 @@
         <v>25</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C291" s="2">
         <v>24</v>
@@ -44862,7 +44864,7 @@
         <v>26</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C292" s="2">
         <v>21</v>
@@ -45014,7 +45016,7 @@
         <v>27</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C293" s="2">
         <v>22</v>
@@ -45166,7 +45168,7 @@
         <v>28</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C294" s="2">
         <v>25</v>
@@ -45318,7 +45320,7 @@
         <v>29</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C295" s="2">
         <v>24</v>
@@ -45470,7 +45472,7 @@
         <v>30</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C296" s="2">
         <v>23</v>
@@ -45622,7 +45624,7 @@
         <v>31</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C297" s="2">
         <v>24</v>
@@ -45774,7 +45776,7 @@
         <v>32</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C298" s="2">
         <v>24</v>
@@ -45926,7 +45928,7 @@
         <v>33</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C299" s="2">
         <v>23</v>
@@ -46078,7 +46080,7 @@
         <v>34</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C300" s="2">
         <v>19</v>
@@ -46230,7 +46232,7 @@
         <v>35</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C301" s="2">
         <v>23</v>
@@ -46382,7 +46384,7 @@
         <v>36</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C302" s="2">
         <v>25</v>

</xml_diff>